<commit_message>
Python/Scraper: Scrape data faster, and format data and excel sheet
</commit_message>
<xml_diff>
--- a/pokemon_ou_usage.xlsx
+++ b/pokemon_ou_usage.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,6 +25,7 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -34,7 +35,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,15 +43,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border/>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="percent" xfId="1" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,13 +418,17 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B26"/>
+  <dimension ref="A1:B73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="23.5" customWidth="1" min="1" max="1"/>
+    <col width="25.5" customWidth="1" min="2" max="2"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -439,10 +448,8 @@
           <t>Kingambit</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>34.52%</t>
-        </is>
+      <c r="B2" s="1" t="n">
+        <v>0.3452</v>
       </c>
     </row>
     <row r="3">
@@ -451,10 +458,8 @@
           <t>Great Tusk</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>33.71%</t>
-        </is>
+      <c r="B3" s="1" t="n">
+        <v>0.3371</v>
       </c>
     </row>
     <row r="4">
@@ -463,10 +468,8 @@
           <t>Landorus-Therian</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>30.49%</t>
-        </is>
+      <c r="B4" s="1" t="n">
+        <v>0.3049</v>
       </c>
     </row>
     <row r="5">
@@ -475,10 +478,8 @@
           <t>Slowking-Galar</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>26.60%</t>
-        </is>
+      <c r="B5" s="1" t="n">
+        <v>0.266</v>
       </c>
     </row>
     <row r="6">
@@ -487,10 +488,8 @@
           <t>Raging Bolt</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>23.83%</t>
-        </is>
+      <c r="B6" s="1" t="n">
+        <v>0.2383</v>
       </c>
     </row>
     <row r="7">
@@ -499,10 +498,8 @@
           <t>Zamazenta</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>20.91%</t>
-        </is>
+      <c r="B7" s="1" t="n">
+        <v>0.2091</v>
       </c>
     </row>
     <row r="8">
@@ -511,10 +508,8 @@
           <t>Gholdengo</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>19.29%</t>
-        </is>
+      <c r="B8" s="1" t="n">
+        <v>0.1929</v>
       </c>
     </row>
     <row r="9">
@@ -523,10 +518,8 @@
           <t>Ogerpon-Wellspring</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>18.70%</t>
-        </is>
+      <c r="B9" s="1" t="n">
+        <v>0.187</v>
       </c>
     </row>
     <row r="10">
@@ -535,10 +528,8 @@
           <t>Iron Moth</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>18.34%</t>
-        </is>
+      <c r="B10" s="1" t="n">
+        <v>0.1834</v>
       </c>
     </row>
     <row r="11">
@@ -547,10 +538,8 @@
           <t>Gliscor</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>17.88%</t>
-        </is>
+      <c r="B11" s="1" t="n">
+        <v>0.1788</v>
       </c>
     </row>
     <row r="12">
@@ -559,10 +548,8 @@
           <t>Roaring Moon</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>17.21%</t>
-        </is>
+      <c r="B12" s="1" t="n">
+        <v>0.1721</v>
       </c>
     </row>
     <row r="13">
@@ -571,10 +558,8 @@
           <t>Samurott-Hisui</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>16.06%</t>
-        </is>
+      <c r="B13" s="1" t="n">
+        <v>0.1606</v>
       </c>
     </row>
     <row r="14">
@@ -583,10 +568,8 @@
           <t>Kyurem</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>15.83%</t>
-        </is>
+      <c r="B14" s="1" t="n">
+        <v>0.1583</v>
       </c>
     </row>
     <row r="15">
@@ -595,10 +578,8 @@
           <t>Dragapult</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>13.05%</t>
-        </is>
+      <c r="B15" s="1" t="n">
+        <v>0.1305</v>
       </c>
     </row>
     <row r="16">
@@ -607,10 +588,8 @@
           <t>Ting-Lu</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>12.39%</t>
-        </is>
+      <c r="B16" s="1" t="n">
+        <v>0.1239</v>
       </c>
     </row>
     <row r="17">
@@ -619,10 +598,8 @@
           <t>Iron Valiant</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>12.37%</t>
-        </is>
+      <c r="B17" s="1" t="n">
+        <v>0.1237</v>
       </c>
     </row>
     <row r="18">
@@ -631,10 +608,8 @@
           <t>Gouging Fire</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>11.65%</t>
-        </is>
+      <c r="B18" s="1" t="n">
+        <v>0.1165</v>
       </c>
     </row>
     <row r="19">
@@ -643,10 +618,8 @@
           <t>Darkrai</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>11.21%</t>
-        </is>
+      <c r="B19" s="1" t="n">
+        <v>0.1121</v>
       </c>
     </row>
     <row r="20">
@@ -655,10 +628,8 @@
           <t>Primarina</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>11.05%</t>
-        </is>
+      <c r="B20" s="1" t="n">
+        <v>0.1105</v>
       </c>
     </row>
     <row r="21">
@@ -667,10 +638,8 @@
           <t>Dragonite</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>10.80%</t>
-        </is>
+      <c r="B21" s="1" t="n">
+        <v>0.108</v>
       </c>
     </row>
     <row r="22">
@@ -679,10 +648,8 @@
           <t>Glimmora</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>10.04%</t>
-        </is>
+      <c r="B22" s="1" t="n">
+        <v>0.1004</v>
       </c>
     </row>
     <row r="23">
@@ -691,10 +658,8 @@
           <t>Cinderace</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>9.87%</t>
-        </is>
+      <c r="B23" s="1" t="n">
+        <v>0.0987</v>
       </c>
     </row>
     <row r="24">
@@ -703,10 +668,8 @@
           <t>Corviknight</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>9.76%</t>
-        </is>
+      <c r="B24" s="1" t="n">
+        <v>0.09759999999999999</v>
       </c>
     </row>
     <row r="25">
@@ -715,10 +678,8 @@
           <t>Moltres</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>8.83%</t>
-        </is>
+      <c r="B25" s="1" t="n">
+        <v>0.0883</v>
       </c>
     </row>
     <row r="26">
@@ -727,10 +688,478 @@
           <t>Iron Crown</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>7.78%</t>
-        </is>
+      <c r="B26" s="1" t="n">
+        <v>0.07780000000000001</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Garganacl</t>
+        </is>
+      </c>
+      <c r="B27" s="1" t="n">
+        <v>0.07580000000000001</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Enamorus</t>
+        </is>
+      </c>
+      <c r="B28" s="1" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Alomomola</t>
+        </is>
+      </c>
+      <c r="B29" s="1" t="n">
+        <v>0.06950000000000001</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Clefable</t>
+        </is>
+      </c>
+      <c r="B30" s="1" t="n">
+        <v>0.06909999999999999</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Weavile</t>
+        </is>
+      </c>
+      <c r="B31" s="1" t="n">
+        <v>0.0673</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Zapdos</t>
+        </is>
+      </c>
+      <c r="B32" s="1" t="n">
+        <v>0.0633</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Deoxys-Speed</t>
+        </is>
+      </c>
+      <c r="B33" s="1" t="n">
+        <v>0.0622</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Dondozo</t>
+        </is>
+      </c>
+      <c r="B34" s="1" t="n">
+        <v>0.0573</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Tinkaton</t>
+        </is>
+      </c>
+      <c r="B35" s="1" t="n">
+        <v>0.0552</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Blissey</t>
+        </is>
+      </c>
+      <c r="B36" s="1" t="n">
+        <v>0.0546</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Skarmory</t>
+        </is>
+      </c>
+      <c r="B37" s="1" t="n">
+        <v>0.0539</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Iron Treads</t>
+        </is>
+      </c>
+      <c r="B38" s="1" t="n">
+        <v>0.0519</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Walking Wake</t>
+        </is>
+      </c>
+      <c r="B39" s="1" t="n">
+        <v>0.0443</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Sinistcha</t>
+        </is>
+      </c>
+      <c r="B40" s="1" t="n">
+        <v>0.0441</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Toxapex</t>
+        </is>
+      </c>
+      <c r="B41" s="1" t="n">
+        <v>0.044</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Ogerpon</t>
+        </is>
+      </c>
+      <c r="B42" s="1" t="n">
+        <v>0.0426</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Clodsire</t>
+        </is>
+      </c>
+      <c r="B43" s="1" t="n">
+        <v>0.0403</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Hatterene</t>
+        </is>
+      </c>
+      <c r="B44" s="1" t="n">
+        <v>0.0401</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Meowscarada</t>
+        </is>
+      </c>
+      <c r="B45" s="1" t="n">
+        <v>0.0386</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Rillaboom</t>
+        </is>
+      </c>
+      <c r="B46" s="1" t="n">
+        <v>0.0349</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Weezing-Galar</t>
+        </is>
+      </c>
+      <c r="B47" s="1" t="n">
+        <v>0.0321</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Lokix</t>
+        </is>
+      </c>
+      <c r="B48" s="1" t="n">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Ribombee</t>
+        </is>
+      </c>
+      <c r="B49" s="1" t="n">
+        <v>0.025</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Heatran</t>
+        </is>
+      </c>
+      <c r="B50" s="1" t="n">
+        <v>0.0237</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Scizor</t>
+        </is>
+      </c>
+      <c r="B51" s="1" t="n">
+        <v>0.0223</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Hydrapple</t>
+        </is>
+      </c>
+      <c r="B52" s="1" t="n">
+        <v>0.0188</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Torkoal</t>
+        </is>
+      </c>
+      <c r="B53" s="1" t="n">
+        <v>0.0178</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Hoopa-Unbound</t>
+        </is>
+      </c>
+      <c r="B54" s="1" t="n">
+        <v>0.0174</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Keldeo</t>
+        </is>
+      </c>
+      <c r="B55" s="1" t="n">
+        <v>0.0173</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Slither Wing</t>
+        </is>
+      </c>
+      <c r="B56" s="1" t="n">
+        <v>0.0159</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Ninetales</t>
+        </is>
+      </c>
+      <c r="B57" s="1" t="n">
+        <v>0.0159</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Enamorus-Therian</t>
+        </is>
+      </c>
+      <c r="B58" s="1" t="n">
+        <v>0.0156</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Excadrill</t>
+        </is>
+      </c>
+      <c r="B59" s="1" t="n">
+        <v>0.0156</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Pelipper</t>
+        </is>
+      </c>
+      <c r="B60" s="1" t="n">
+        <v>0.0148</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Amoonguss</t>
+        </is>
+      </c>
+      <c r="B61" s="1" t="n">
+        <v>0.0147</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Skeledirge</t>
+        </is>
+      </c>
+      <c r="B62" s="1" t="n">
+        <v>0.0143</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Ninetales-Alola</t>
+        </is>
+      </c>
+      <c r="B63" s="1" t="n">
+        <v>0.0142</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Tyranitar</t>
+        </is>
+      </c>
+      <c r="B64" s="1" t="n">
+        <v>0.0141</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Iron Boulder</t>
+        </is>
+      </c>
+      <c r="B65" s="1" t="n">
+        <v>0.014</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Goodra-Hisui</t>
+        </is>
+      </c>
+      <c r="B66" s="1" t="n">
+        <v>0.0138</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Mandibuzz</t>
+        </is>
+      </c>
+      <c r="B67" s="1" t="n">
+        <v>0.0136</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Ursaluna</t>
+        </is>
+      </c>
+      <c r="B68" s="1" t="n">
+        <v>0.0132</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Pecharunt</t>
+        </is>
+      </c>
+      <c r="B69" s="1" t="n">
+        <v>0.0131</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Manaphy</t>
+        </is>
+      </c>
+      <c r="B70" s="1" t="n">
+        <v>0.0128</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Serperior</t>
+        </is>
+      </c>
+      <c r="B71" s="1" t="n">
+        <v>0.0127</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Quagsire</t>
+        </is>
+      </c>
+      <c r="B72" s="1" t="n">
+        <v>0.0126</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Hydreigon</t>
+        </is>
+      </c>
+      <c r="B73" s="1" t="n">
+        <v>0.0123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update page being scraped and add additional document format
</commit_message>
<xml_diff>
--- a/pokemon_ou_usage.xlsx
+++ b/pokemon_ou_usage.xlsx
@@ -418,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B73"/>
+  <dimension ref="A1:B69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,7 +426,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="23.5" customWidth="1" min="1" max="1"/>
+    <col width="25.5" customWidth="1" min="1" max="1"/>
     <col width="25.5" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
@@ -445,627 +445,627 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Kingambit</t>
+          <t>Landorus-Therian</t>
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>0.3452</v>
+        <v>0.2997</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Great Tusk</t>
+          <t>Garchomp</t>
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>0.3371</v>
+        <v>0.2992</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Landorus-Therian</t>
+          <t>Ferrothorn</t>
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>0.3049</v>
+        <v>0.2758</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Slowking-Galar</t>
+          <t>Zapdos</t>
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>0.266</v>
+        <v>0.2692</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Raging Bolt</t>
+          <t>Dragapult</t>
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>0.2383</v>
+        <v>0.2591</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Zamazenta</t>
+          <t>Weavile</t>
         </is>
       </c>
       <c r="B7" s="1" t="n">
-        <v>0.2091</v>
+        <v>0.2582</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Gholdengo</t>
+          <t>Heatran</t>
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.1929</v>
+        <v>0.2467</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Ogerpon-Wellspring</t>
+          <t>Clefable</t>
         </is>
       </c>
       <c r="B9" s="1" t="n">
-        <v>0.187</v>
+        <v>0.2265</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Iron Moth</t>
+          <t>Rillaboom</t>
         </is>
       </c>
       <c r="B10" s="1" t="n">
-        <v>0.1834</v>
+        <v>0.1974</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Gliscor</t>
+          <t>Tapu Lele</t>
         </is>
       </c>
       <c r="B11" s="1" t="n">
-        <v>0.1788</v>
+        <v>0.1904</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Roaring Moon</t>
+          <t>Tornadus-Therian</t>
         </is>
       </c>
       <c r="B12" s="1" t="n">
-        <v>0.1721</v>
+        <v>0.1869</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Samurott-Hisui</t>
+          <t>Urshifu-Rapid-Strike</t>
         </is>
       </c>
       <c r="B13" s="1" t="n">
-        <v>0.1606</v>
+        <v>0.1831</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Kyurem</t>
+          <t>Melmetal</t>
         </is>
       </c>
       <c r="B14" s="1" t="n">
-        <v>0.1583</v>
+        <v>0.1767</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Dragapult</t>
+          <t>Kartana</t>
         </is>
       </c>
       <c r="B15" s="1" t="n">
-        <v>0.1305</v>
+        <v>0.1646</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Ting-Lu</t>
+          <t>Slowbro</t>
         </is>
       </c>
       <c r="B16" s="1" t="n">
-        <v>0.1239</v>
+        <v>0.1569</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Iron Valiant</t>
+          <t>Tyranitar</t>
         </is>
       </c>
       <c r="B17" s="1" t="n">
-        <v>0.1237</v>
+        <v>0.1278</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Gouging Fire</t>
+          <t>Excadrill</t>
         </is>
       </c>
       <c r="B18" s="1" t="n">
-        <v>0.1165</v>
+        <v>0.117</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Darkrai</t>
+          <t>Toxapex</t>
         </is>
       </c>
       <c r="B19" s="1" t="n">
-        <v>0.1121</v>
+        <v>0.1166</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Primarina</t>
+          <t>Corviknight</t>
         </is>
       </c>
       <c r="B20" s="1" t="n">
-        <v>0.1105</v>
+        <v>0.1151</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Dragonite</t>
+          <t>Hatterene</t>
         </is>
       </c>
       <c r="B21" s="1" t="n">
-        <v>0.108</v>
+        <v>0.1102</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Glimmora</t>
+          <t>Blaziken</t>
         </is>
       </c>
       <c r="B22" s="1" t="n">
-        <v>0.1004</v>
+        <v>0.1064</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Cinderace</t>
+          <t>Zeraora</t>
         </is>
       </c>
       <c r="B23" s="1" t="n">
-        <v>0.0987</v>
+        <v>0.08529999999999999</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Corviknight</t>
+          <t>Slowking-Galar</t>
         </is>
       </c>
       <c r="B24" s="1" t="n">
-        <v>0.09759999999999999</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Moltres</t>
+          <t>Tapu Koko</t>
         </is>
       </c>
       <c r="B25" s="1" t="n">
-        <v>0.0883</v>
+        <v>0.0784</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Iron Crown</t>
+          <t>Tapu Fini</t>
         </is>
       </c>
       <c r="B26" s="1" t="n">
-        <v>0.07780000000000001</v>
+        <v>0.06860000000000001</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Garganacl</t>
+          <t>Blacephalon</t>
         </is>
       </c>
       <c r="B27" s="1" t="n">
-        <v>0.07580000000000001</v>
+        <v>0.0668</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Enamorus</t>
+          <t>Rotom-Wash</t>
         </is>
       </c>
       <c r="B28" s="1" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.06509999999999999</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Alomomola</t>
+          <t>Dragonite</t>
         </is>
       </c>
       <c r="B29" s="1" t="n">
-        <v>0.06950000000000001</v>
+        <v>0.0623</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Clefable</t>
+          <t>Mew</t>
         </is>
       </c>
       <c r="B30" s="1" t="n">
-        <v>0.06909999999999999</v>
+        <v>0.0607</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Weavile</t>
+          <t>Hippowdon</t>
         </is>
       </c>
       <c r="B31" s="1" t="n">
-        <v>0.0673</v>
+        <v>0.0591</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Zapdos</t>
+          <t>Gastrodon</t>
         </is>
       </c>
       <c r="B32" s="1" t="n">
-        <v>0.0633</v>
+        <v>0.0535</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Deoxys-Speed</t>
+          <t>Volcarona</t>
         </is>
       </c>
       <c r="B33" s="1" t="n">
-        <v>0.0622</v>
+        <v>0.0521</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Dondozo</t>
+          <t>Bisharp</t>
         </is>
       </c>
       <c r="B34" s="1" t="n">
-        <v>0.0573</v>
+        <v>0.0517</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Tinkaton</t>
+          <t>Skarmory</t>
         </is>
       </c>
       <c r="B35" s="1" t="n">
-        <v>0.0552</v>
+        <v>0.049</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Blissey</t>
+          <t>Marowak-Alola</t>
         </is>
       </c>
       <c r="B36" s="1" t="n">
-        <v>0.0546</v>
+        <v>0.04849999999999999</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Skarmory</t>
+          <t>Magnezone</t>
         </is>
       </c>
       <c r="B37" s="1" t="n">
-        <v>0.0539</v>
+        <v>0.0472</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Iron Treads</t>
+          <t>Drampa</t>
         </is>
       </c>
       <c r="B38" s="1" t="n">
-        <v>0.0519</v>
+        <v>0.044</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Walking Wake</t>
+          <t>Buzzwole</t>
         </is>
       </c>
       <c r="B39" s="1" t="n">
-        <v>0.0443</v>
+        <v>0.0426</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Sinistcha</t>
+          <t>Victini</t>
         </is>
       </c>
       <c r="B40" s="1" t="n">
-        <v>0.0441</v>
+        <v>0.0394</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Toxapex</t>
+          <t>Blissey</t>
         </is>
       </c>
       <c r="B41" s="1" t="n">
-        <v>0.044</v>
+        <v>0.0372</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Ogerpon</t>
+          <t>Pelipper</t>
         </is>
       </c>
       <c r="B42" s="1" t="n">
-        <v>0.0426</v>
+        <v>0.0359</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Clodsire</t>
+          <t>Stakataka</t>
         </is>
       </c>
       <c r="B43" s="1" t="n">
-        <v>0.0403</v>
+        <v>0.0354</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Hatterene</t>
+          <t>Scizor</t>
         </is>
       </c>
       <c r="B44" s="1" t="n">
-        <v>0.0401</v>
+        <v>0.0352</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Meowscarada</t>
+          <t>Nidoking</t>
         </is>
       </c>
       <c r="B45" s="1" t="n">
-        <v>0.0386</v>
+        <v>0.0338</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Rillaboom</t>
+          <t>Ninetales-Alola</t>
         </is>
       </c>
       <c r="B46" s="1" t="n">
-        <v>0.0349</v>
+        <v>0.0335</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Weezing-Galar</t>
+          <t>Barraskewda</t>
         </is>
       </c>
       <c r="B47" s="1" t="n">
-        <v>0.0321</v>
+        <v>0.0312</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Lokix</t>
+          <t>Volcanion</t>
         </is>
       </c>
       <c r="B48" s="1" t="n">
-        <v>0.026</v>
+        <v>0.0266</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Ribombee</t>
+          <t>Slowking</t>
         </is>
       </c>
       <c r="B49" s="1" t="n">
-        <v>0.025</v>
+        <v>0.0253</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Heatran</t>
+          <t>Celesteela</t>
         </is>
       </c>
       <c r="B50" s="1" t="n">
-        <v>0.0237</v>
+        <v>0.0232</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Scizor</t>
+          <t>Moltres-Galar</t>
         </is>
       </c>
       <c r="B51" s="1" t="n">
-        <v>0.0223</v>
+        <v>0.0231</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Hydrapple</t>
+          <t>Aegislash</t>
         </is>
       </c>
       <c r="B52" s="1" t="n">
-        <v>0.0188</v>
+        <v>0.023</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Torkoal</t>
+          <t>Cloyster</t>
         </is>
       </c>
       <c r="B53" s="1" t="n">
-        <v>0.0178</v>
+        <v>0.0225</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Hoopa-Unbound</t>
+          <t>Umbreon</t>
         </is>
       </c>
       <c r="B54" s="1" t="n">
-        <v>0.0174</v>
+        <v>0.0222</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Keldeo</t>
+          <t>Seismitoad</t>
         </is>
       </c>
       <c r="B55" s="1" t="n">
-        <v>0.0173</v>
+        <v>0.0213</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Slither Wing</t>
+          <t>Dracozolt</t>
         </is>
       </c>
       <c r="B56" s="1" t="n">
-        <v>0.0159</v>
+        <v>0.021</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Ninetales</t>
+          <t>Swampert</t>
         </is>
       </c>
       <c r="B57" s="1" t="n">
-        <v>0.0159</v>
+        <v>0.0204</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Enamorus-Therian</t>
+          <t>Regieleki</t>
         </is>
       </c>
       <c r="B58" s="1" t="n">
-        <v>0.0156</v>
+        <v>0.0202</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Excadrill</t>
+          <t>Crawdaunt</t>
         </is>
       </c>
       <c r="B59" s="1" t="n">
-        <v>0.0156</v>
+        <v>0.0201</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Pelipper</t>
+          <t>Hawlucha</t>
         </is>
       </c>
       <c r="B60" s="1" t="n">
-        <v>0.0148</v>
+        <v>0.0199</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Amoonguss</t>
+          <t>Hydreigon</t>
         </is>
       </c>
       <c r="B61" s="1" t="n">
-        <v>0.0147</v>
+        <v>0.0164</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Skeledirge</t>
+          <t>Nihilego</t>
         </is>
       </c>
       <c r="B62" s="1" t="n">
-        <v>0.0143</v>
+        <v>0.0163</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Ninetales-Alola</t>
+          <t>Quagsire</t>
         </is>
       </c>
       <c r="B63" s="1" t="n">
-        <v>0.0142</v>
+        <v>0.0153</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Tyranitar</t>
+          <t>Suicune</t>
         </is>
       </c>
       <c r="B64" s="1" t="n">
@@ -1075,91 +1075,51 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Iron Boulder</t>
+          <t>Arctozolt</t>
         </is>
       </c>
       <c r="B65" s="1" t="n">
-        <v>0.014</v>
+        <v>0.0124</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Goodra-Hisui</t>
+          <t>Moltres</t>
         </is>
       </c>
       <c r="B66" s="1" t="n">
-        <v>0.0138</v>
+        <v>0.0118</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Mandibuzz</t>
+          <t>Porygon2</t>
         </is>
       </c>
       <c r="B67" s="1" t="n">
-        <v>0.0136</v>
+        <v>0.0107</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Ursaluna</t>
+          <t>Zapdos-Galar</t>
         </is>
       </c>
       <c r="B68" s="1" t="n">
-        <v>0.0132</v>
+        <v>0.0104</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Pecharunt</t>
+          <t>Reuniclus</t>
         </is>
       </c>
       <c r="B69" s="1" t="n">
-        <v>0.0131</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>Manaphy</t>
-        </is>
-      </c>
-      <c r="B70" s="1" t="n">
-        <v>0.0128</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>Serperior</t>
-        </is>
-      </c>
-      <c r="B71" s="1" t="n">
-        <v>0.0127</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>Quagsire</t>
-        </is>
-      </c>
-      <c r="B72" s="1" t="n">
-        <v>0.0126</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>Hydreigon</t>
-        </is>
-      </c>
-      <c r="B73" s="1" t="n">
-        <v>0.0123</v>
+        <v>0.0103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>